<commit_message>
Default NH3 for more states added
</commit_message>
<xml_diff>
--- a/Inputs/ertac_additional_variables.xlsx
+++ b/Inputs/ertac_additional_variables.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$158</definedName>
     <definedName name="ertac_additional_variables" localSheetId="0">Sheet1!$A$1:$P$158</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -567,7 +568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -658,7 +661,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J2">
         <v>20100201</v>
@@ -740,7 +743,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J4">
         <v>20100201</v>
@@ -822,7 +825,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J6">
         <v>20100201</v>
@@ -904,7 +907,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J8">
         <v>20100201</v>
@@ -1206,7 +1209,7 @@
         <v>5.2399999999999999E-3</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J15">
         <v>20100201</v>
@@ -1288,7 +1291,7 @@
         <v>2.0699999999999998E-3</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J17">
         <v>20100201</v>
@@ -1329,7 +1332,7 @@
         <v>2.2200000000000002E-3</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J18">
         <v>20100201</v>
@@ -1411,7 +1414,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J20">
         <v>20100201</v>
@@ -1493,7 +1496,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J22">
         <v>20100201</v>
@@ -1534,7 +1537,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J23">
         <v>20100201</v>
@@ -1616,7 +1619,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J25">
         <v>20100201</v>
@@ -1698,7 +1701,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J27">
         <v>20100201</v>
@@ -1739,7 +1742,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J28">
         <v>20100201</v>
@@ -1821,7 +1824,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J30">
         <v>20100201</v>
@@ -1903,7 +1906,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J32">
         <v>20100201</v>
@@ -1944,7 +1947,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J33">
         <v>20100201</v>
@@ -2026,7 +2029,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J35">
         <v>20100201</v>
@@ -2108,7 +2111,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J37">
         <v>20100201</v>
@@ -2149,7 +2152,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J38">
         <v>20100201</v>
@@ -2231,7 +2234,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J40">
         <v>20100201</v>
@@ -2313,7 +2316,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J42">
         <v>20100201</v>
@@ -2354,7 +2357,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J43">
         <v>20100201</v>
@@ -2436,7 +2439,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J45">
         <v>20100201</v>
@@ -2518,7 +2521,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J47">
         <v>20100201</v>
@@ -2559,7 +2562,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J48">
         <v>20100201</v>
@@ -2641,7 +2644,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J50">
         <v>20100201</v>
@@ -2723,7 +2726,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J52">
         <v>20100201</v>
@@ -2764,7 +2767,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J53">
         <v>20100201</v>
@@ -2846,7 +2849,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J55">
         <v>20100201</v>
@@ -2928,7 +2931,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J57">
         <v>20100201</v>
@@ -2969,7 +2972,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J58">
         <v>20100201</v>
@@ -3051,7 +3054,7 @@
         <v>4.3800000000000002E-3</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J60">
         <v>20100201</v>
@@ -3133,7 +3136,7 @@
         <v>2.5699999999999998E-3</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J62">
         <v>20100201</v>
@@ -3174,7 +3177,7 @@
         <v>0.02</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J63">
         <v>20100201</v>
@@ -3256,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J65">
         <v>20100201</v>
@@ -3338,7 +3341,7 @@
         <v>2.0400000000000001E-3</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J67">
         <v>20100201</v>
@@ -3379,7 +3382,7 @@
         <v>4.5399999999999998E-3</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J68">
         <v>20100201</v>
@@ -3461,7 +3464,7 @@
         <v>9.19E-4</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J70">
         <v>20100201</v>
@@ -3502,7 +3505,7 @@
         <v>4.3299999999999996E-3</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J71">
         <v>20100201</v>
@@ -3584,7 +3587,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J73">
         <v>20100201</v>
@@ -3666,7 +3669,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J75">
         <v>20100201</v>
@@ -3707,7 +3710,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J76">
         <v>20100201</v>
@@ -3789,7 +3792,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J78">
         <v>20100201</v>
@@ -3871,7 +3874,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J80">
         <v>20100201</v>
@@ -3953,7 +3956,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J82">
         <v>20100201</v>
@@ -4035,7 +4038,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J84">
         <v>20100201</v>
@@ -4117,7 +4120,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J86">
         <v>20100201</v>
@@ -4199,7 +4202,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J88">
         <v>20100201</v>
@@ -4240,7 +4243,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J89">
         <v>20100201</v>
@@ -4322,7 +4325,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J91">
         <v>20100201</v>
@@ -4404,7 +4407,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J93">
         <v>20100201</v>
@@ -4445,7 +4448,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J94">
         <v>20100201</v>
@@ -4527,7 +4530,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J96">
         <v>20100201</v>
@@ -4609,7 +4612,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J98">
         <v>20100201</v>
@@ -4650,7 +4653,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J99">
         <v>20100201</v>
@@ -4773,7 +4776,7 @@
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J102">
         <v>20100201</v>
@@ -4814,7 +4817,7 @@
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J103">
         <v>20100201</v>
@@ -4855,7 +4858,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J104">
         <v>10100602</v>
@@ -4937,7 +4940,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J106">
         <v>20100201</v>
@@ -4978,7 +4981,7 @@
         <v>0.01</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J107">
         <v>20100101</v>
@@ -5060,7 +5063,7 @@
         <v>5.28E-3</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J109">
         <v>20100201</v>
@@ -5142,7 +5145,7 @@
         <v>0.01</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J111">
         <v>20100201</v>
@@ -5183,7 +5186,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J112">
         <v>20100201</v>
@@ -5306,7 +5309,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J115">
         <v>20100201</v>
@@ -5347,7 +5350,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G116">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J116">
         <v>20100201</v>
@@ -5429,7 +5432,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G118">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J118">
         <v>20100201</v>
@@ -5511,7 +5514,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J120">
         <v>20100201</v>
@@ -5552,7 +5555,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J121">
         <v>20100201</v>
@@ -5634,7 +5637,7 @@
         <v>3.4399999999999999E-3</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J123">
         <v>20100201</v>
@@ -5716,7 +5719,7 @@
         <v>0.01</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J125">
         <v>20100201</v>
@@ -5757,7 +5760,7 @@
         <v>1.49E-3</v>
       </c>
       <c r="G126">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J126">
         <v>20100201</v>
@@ -5883,7 +5886,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G129">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J129">
         <v>20100201</v>
@@ -5965,7 +5968,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G131">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J131">
         <v>20100201</v>
@@ -6006,7 +6009,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G132">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J132">
         <v>20100201</v>
@@ -6088,7 +6091,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G134">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J134">
         <v>20100201</v>
@@ -6129,7 +6132,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J135">
         <v>20100201</v>
@@ -6211,7 +6214,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G137">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J137">
         <v>20100201</v>
@@ -6293,7 +6296,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G139">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J139">
         <v>20100201</v>
@@ -6375,7 +6378,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J141">
         <v>20100201</v>
@@ -6416,7 +6419,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G142">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J142">
         <v>20100201</v>
@@ -6498,7 +6501,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="G144">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J144">
         <v>20100201</v>
@@ -6580,7 +6583,7 @@
         <v>1.6800000000000001E-3</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J146">
         <v>20100201</v>
@@ -6621,7 +6624,7 @@
         <v>3.8600000000000001E-3</v>
       </c>
       <c r="G147">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J147">
         <v>20100201</v>
@@ -6703,7 +6706,7 @@
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J149">
         <v>20100201</v>
@@ -6744,7 +6747,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G150">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J150">
         <v>20100201</v>
@@ -6826,7 +6829,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J152">
         <v>20100201</v>
@@ -6867,7 +6870,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G153">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J153">
         <v>20100201</v>
@@ -6949,7 +6952,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G155">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J155">
         <v>20100201</v>
@@ -7031,7 +7034,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J157">
         <v>20100201</v>

</xml_diff>

<commit_message>
Revert "Default NH3 for more states added"
This reverts commit 4a780cf692e7cdb61e1a3f8ce6607f48002754b8.
</commit_message>
<xml_diff>
--- a/Inputs/ertac_additional_variables.xlsx
+++ b/Inputs/ertac_additional_variables.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$158</definedName>
     <definedName name="ertac_additional_variables" localSheetId="0">Sheet1!$A$1:$P$158</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -568,9 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -661,7 +658,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G2">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>20100201</v>
@@ -743,7 +740,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G4">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>20100201</v>
@@ -825,7 +822,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G6">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>20100201</v>
@@ -907,7 +904,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G8">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>20100201</v>
@@ -1209,7 +1206,7 @@
         <v>5.2399999999999999E-3</v>
       </c>
       <c r="G15">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>20100201</v>
@@ -1291,7 +1288,7 @@
         <v>2.0699999999999998E-3</v>
       </c>
       <c r="G17">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>20100201</v>
@@ -1332,7 +1329,7 @@
         <v>2.2200000000000002E-3</v>
       </c>
       <c r="G18">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>20100201</v>
@@ -1414,7 +1411,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G20">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>20100201</v>
@@ -1496,7 +1493,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G22">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>20100201</v>
@@ -1537,7 +1534,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G23">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>20100201</v>
@@ -1619,7 +1616,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G25">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>20100201</v>
@@ -1701,7 +1698,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G27">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <v>20100201</v>
@@ -1742,7 +1739,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G28">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>20100201</v>
@@ -1824,7 +1821,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G30">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>20100201</v>
@@ -1906,7 +1903,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G32">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J32">
         <v>20100201</v>
@@ -1947,7 +1944,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G33">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <v>20100201</v>
@@ -2029,7 +2026,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G35">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>20100201</v>
@@ -2111,7 +2108,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G37">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <v>20100201</v>
@@ -2152,7 +2149,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G38">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <v>20100201</v>
@@ -2234,7 +2231,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G40">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>20100201</v>
@@ -2316,7 +2313,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G42">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <v>20100201</v>
@@ -2357,7 +2354,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G43">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>20100201</v>
@@ -2439,7 +2436,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G45">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J45">
         <v>20100201</v>
@@ -2521,7 +2518,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G47">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J47">
         <v>20100201</v>
@@ -2562,7 +2559,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G48">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J48">
         <v>20100201</v>
@@ -2644,7 +2641,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G50">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J50">
         <v>20100201</v>
@@ -2726,7 +2723,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G52">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J52">
         <v>20100201</v>
@@ -2767,7 +2764,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G53">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J53">
         <v>20100201</v>
@@ -2849,7 +2846,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G55">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J55">
         <v>20100201</v>
@@ -2931,7 +2928,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G57">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J57">
         <v>20100201</v>
@@ -2972,7 +2969,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G58">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J58">
         <v>20100201</v>
@@ -3054,7 +3051,7 @@
         <v>4.3800000000000002E-3</v>
       </c>
       <c r="G60">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J60">
         <v>20100201</v>
@@ -3136,7 +3133,7 @@
         <v>2.5699999999999998E-3</v>
       </c>
       <c r="G62">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <v>20100201</v>
@@ -3177,7 +3174,7 @@
         <v>0.02</v>
       </c>
       <c r="G63">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J63">
         <v>20100201</v>
@@ -3259,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J65">
         <v>20100201</v>
@@ -3341,7 +3338,7 @@
         <v>2.0400000000000001E-3</v>
       </c>
       <c r="G67">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J67">
         <v>20100201</v>
@@ -3382,7 +3379,7 @@
         <v>4.5399999999999998E-3</v>
       </c>
       <c r="G68">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J68">
         <v>20100201</v>
@@ -3464,7 +3461,7 @@
         <v>9.19E-4</v>
       </c>
       <c r="G70">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J70">
         <v>20100201</v>
@@ -3505,7 +3502,7 @@
         <v>4.3299999999999996E-3</v>
       </c>
       <c r="G71">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J71">
         <v>20100201</v>
@@ -3587,7 +3584,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G73">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J73">
         <v>20100201</v>
@@ -3669,7 +3666,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G75">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J75">
         <v>20100201</v>
@@ -3710,7 +3707,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G76">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J76">
         <v>20100201</v>
@@ -3792,7 +3789,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G78">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J78">
         <v>20100201</v>
@@ -3874,7 +3871,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G80">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J80">
         <v>20100201</v>
@@ -3956,7 +3953,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G82">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J82">
         <v>20100201</v>
@@ -4038,7 +4035,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G84">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J84">
         <v>20100201</v>
@@ -4120,7 +4117,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G86">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J86">
         <v>20100201</v>
@@ -4202,7 +4199,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G88">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J88">
         <v>20100201</v>
@@ -4243,7 +4240,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G89">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J89">
         <v>20100201</v>
@@ -4325,7 +4322,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G91">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J91">
         <v>20100201</v>
@@ -4407,7 +4404,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G93">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J93">
         <v>20100201</v>
@@ -4448,7 +4445,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G94">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J94">
         <v>20100201</v>
@@ -4530,7 +4527,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G96">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J96">
         <v>20100201</v>
@@ -4612,7 +4609,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G98">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J98">
         <v>20100201</v>
@@ -4653,7 +4650,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G99">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J99">
         <v>20100201</v>
@@ -4776,7 +4773,7 @@
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="G102">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J102">
         <v>20100201</v>
@@ -4817,7 +4814,7 @@
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="G103">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J103">
         <v>20100201</v>
@@ -4858,7 +4855,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="G104">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J104">
         <v>10100602</v>
@@ -4940,7 +4937,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G106">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J106">
         <v>20100201</v>
@@ -4981,7 +4978,7 @@
         <v>0.01</v>
       </c>
       <c r="G107">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J107">
         <v>20100101</v>
@@ -5063,7 +5060,7 @@
         <v>5.28E-3</v>
       </c>
       <c r="G109">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J109">
         <v>20100201</v>
@@ -5145,7 +5142,7 @@
         <v>0.01</v>
       </c>
       <c r="G111">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J111">
         <v>20100201</v>
@@ -5186,7 +5183,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
       <c r="G112">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J112">
         <v>20100201</v>
@@ -5309,7 +5306,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G115">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J115">
         <v>20100201</v>
@@ -5350,7 +5347,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G116">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J116">
         <v>20100201</v>
@@ -5432,7 +5429,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G118">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J118">
         <v>20100201</v>
@@ -5514,7 +5511,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G120">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J120">
         <v>20100201</v>
@@ -5555,7 +5552,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G121">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J121">
         <v>20100201</v>
@@ -5637,7 +5634,7 @@
         <v>3.4399999999999999E-3</v>
       </c>
       <c r="G123">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J123">
         <v>20100201</v>
@@ -5719,7 +5716,7 @@
         <v>0.01</v>
       </c>
       <c r="G125">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J125">
         <v>20100201</v>
@@ -5760,7 +5757,7 @@
         <v>1.49E-3</v>
       </c>
       <c r="G126">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J126">
         <v>20100201</v>
@@ -5886,7 +5883,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G129">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J129">
         <v>20100201</v>
@@ -5968,7 +5965,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G131">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J131">
         <v>20100201</v>
@@ -6009,7 +6006,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G132">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J132">
         <v>20100201</v>
@@ -6091,7 +6088,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G134">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J134">
         <v>20100201</v>
@@ -6132,7 +6129,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G135">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J135">
         <v>20100201</v>
@@ -6214,7 +6211,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G137">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J137">
         <v>20100201</v>
@@ -6296,7 +6293,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G139">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J139">
         <v>20100201</v>
@@ -6378,7 +6375,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G141">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J141">
         <v>20100201</v>
@@ -6419,7 +6416,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G142">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J142">
         <v>20100201</v>
@@ -6501,7 +6498,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="G144">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J144">
         <v>20100201</v>
@@ -6583,7 +6580,7 @@
         <v>1.6800000000000001E-3</v>
       </c>
       <c r="G146">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J146">
         <v>20100201</v>
@@ -6624,7 +6621,7 @@
         <v>3.8600000000000001E-3</v>
       </c>
       <c r="G147">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J147">
         <v>20100201</v>
@@ -6706,7 +6703,7 @@
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="G149">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J149">
         <v>20100201</v>
@@ -6747,7 +6744,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G150">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J150">
         <v>20100201</v>
@@ -6829,7 +6826,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G152">
-        <v>3.4400000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="J152">
         <v>20100201</v>
@@ -6870,7 +6867,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G153">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J153">
         <v>20100201</v>
@@ -6952,7 +6949,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G155">
-        <v>3.14E-3</v>
+        <v>0</v>
       </c>
       <c r="J155">
         <v>20100201</v>
@@ -7034,7 +7031,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G157">
-        <v>5.2900000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J157">
         <v>20100201</v>

</xml_diff>

<commit_message>
Default NH3 added for more states
Uses CT values for defaults
</commit_message>
<xml_diff>
--- a/Inputs/ertac_additional_variables.xlsx
+++ b/Inputs/ertac_additional_variables.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$158</definedName>
     <definedName name="ertac_additional_variables" localSheetId="0">Sheet1!$A$1:$P$158</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -567,7 +568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -658,7 +661,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J2">
         <v>20100201</v>
@@ -740,7 +743,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J4">
         <v>20100201</v>
@@ -822,7 +825,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J6">
         <v>20100201</v>
@@ -904,7 +907,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J8">
         <v>20100201</v>
@@ -1206,7 +1209,7 @@
         <v>5.2399999999999999E-3</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J15">
         <v>20100201</v>
@@ -1288,7 +1291,7 @@
         <v>2.0699999999999998E-3</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J17">
         <v>20100201</v>
@@ -1329,7 +1332,7 @@
         <v>2.2200000000000002E-3</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J18">
         <v>20100201</v>
@@ -1411,7 +1414,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J20">
         <v>20100201</v>
@@ -1493,7 +1496,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J22">
         <v>20100201</v>
@@ -1534,7 +1537,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J23">
         <v>20100201</v>
@@ -1616,7 +1619,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J25">
         <v>20100201</v>
@@ -1698,7 +1701,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J27">
         <v>20100201</v>
@@ -1739,7 +1742,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J28">
         <v>20100201</v>
@@ -1821,7 +1824,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J30">
         <v>20100201</v>
@@ -1903,7 +1906,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J32">
         <v>20100201</v>
@@ -1944,7 +1947,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J33">
         <v>20100201</v>
@@ -2026,7 +2029,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J35">
         <v>20100201</v>
@@ -2108,7 +2111,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J37">
         <v>20100201</v>
@@ -2149,7 +2152,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J38">
         <v>20100201</v>
@@ -2231,7 +2234,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J40">
         <v>20100201</v>
@@ -2313,7 +2316,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J42">
         <v>20100201</v>
@@ -2354,7 +2357,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J43">
         <v>20100201</v>
@@ -2436,7 +2439,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J45">
         <v>20100201</v>
@@ -2518,7 +2521,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J47">
         <v>20100201</v>
@@ -2559,7 +2562,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J48">
         <v>20100201</v>
@@ -2641,7 +2644,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J50">
         <v>20100201</v>
@@ -2723,7 +2726,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J52">
         <v>20100201</v>
@@ -2764,7 +2767,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J53">
         <v>20100201</v>
@@ -2846,7 +2849,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J55">
         <v>20100201</v>
@@ -2928,7 +2931,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J57">
         <v>20100201</v>
@@ -2969,7 +2972,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J58">
         <v>20100201</v>
@@ -3051,7 +3054,7 @@
         <v>4.3800000000000002E-3</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J60">
         <v>20100201</v>
@@ -3133,7 +3136,7 @@
         <v>2.5699999999999998E-3</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J62">
         <v>20100201</v>
@@ -3174,7 +3177,7 @@
         <v>0.02</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J63">
         <v>20100201</v>
@@ -3256,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J65">
         <v>20100201</v>
@@ -3338,7 +3341,7 @@
         <v>2.0400000000000001E-3</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J67">
         <v>20100201</v>
@@ -3379,7 +3382,7 @@
         <v>4.5399999999999998E-3</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J68">
         <v>20100201</v>
@@ -3461,7 +3464,7 @@
         <v>9.19E-4</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J70">
         <v>20100201</v>
@@ -3502,7 +3505,7 @@
         <v>4.3299999999999996E-3</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J71">
         <v>20100201</v>
@@ -3584,7 +3587,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J73">
         <v>20100201</v>
@@ -3666,7 +3669,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J75">
         <v>20100201</v>
@@ -3707,7 +3710,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J76">
         <v>20100201</v>
@@ -3789,7 +3792,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J78">
         <v>20100201</v>
@@ -3871,7 +3874,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J80">
         <v>20100201</v>
@@ -3953,7 +3956,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J82">
         <v>20100201</v>
@@ -4035,7 +4038,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J84">
         <v>20100201</v>
@@ -4117,7 +4120,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J86">
         <v>20100201</v>
@@ -4199,7 +4202,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J88">
         <v>20100201</v>
@@ -4240,7 +4243,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J89">
         <v>20100201</v>
@@ -4322,7 +4325,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J91">
         <v>20100201</v>
@@ -4404,7 +4407,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J93">
         <v>20100201</v>
@@ -4445,7 +4448,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J94">
         <v>20100201</v>
@@ -4527,7 +4530,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J96">
         <v>20100201</v>
@@ -4609,7 +4612,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J98">
         <v>20100201</v>
@@ -4650,7 +4653,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J99">
         <v>20100201</v>
@@ -4773,7 +4776,7 @@
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J102">
         <v>20100201</v>
@@ -4814,7 +4817,7 @@
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J103">
         <v>20100201</v>
@@ -4855,7 +4858,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J104">
         <v>10100602</v>
@@ -4937,7 +4940,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J106">
         <v>20100201</v>
@@ -4978,7 +4981,7 @@
         <v>0.01</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J107">
         <v>20100101</v>
@@ -5060,7 +5063,7 @@
         <v>5.28E-3</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J109">
         <v>20100201</v>
@@ -5142,7 +5145,7 @@
         <v>0.01</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J111">
         <v>20100201</v>
@@ -5183,7 +5186,7 @@
         <v>2.7499999999999998E-3</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J112">
         <v>20100201</v>
@@ -5306,7 +5309,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J115">
         <v>20100201</v>
@@ -5347,7 +5350,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G116">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J116">
         <v>20100201</v>
@@ -5429,7 +5432,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G118">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J118">
         <v>20100201</v>
@@ -5511,7 +5514,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J120">
         <v>20100201</v>
@@ -5552,7 +5555,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J121">
         <v>20100201</v>
@@ -5634,7 +5637,7 @@
         <v>3.4399999999999999E-3</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J123">
         <v>20100201</v>
@@ -5716,7 +5719,7 @@
         <v>0.01</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J125">
         <v>20100201</v>
@@ -5757,7 +5760,7 @@
         <v>1.49E-3</v>
       </c>
       <c r="G126">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J126">
         <v>20100201</v>
@@ -5883,7 +5886,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G129">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J129">
         <v>20100201</v>
@@ -5965,7 +5968,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G131">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J131">
         <v>20100201</v>
@@ -6006,7 +6009,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G132">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J132">
         <v>20100201</v>
@@ -6088,7 +6091,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G134">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J134">
         <v>20100201</v>
@@ -6129,7 +6132,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J135">
         <v>20100201</v>
@@ -6211,7 +6214,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G137">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J137">
         <v>20100201</v>
@@ -6293,7 +6296,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G139">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J139">
         <v>20100201</v>
@@ -6375,7 +6378,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J141">
         <v>20100201</v>
@@ -6416,7 +6419,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G142">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J142">
         <v>20100201</v>
@@ -6498,7 +6501,7 @@
         <v>2.82E-3</v>
       </c>
       <c r="G144">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J144">
         <v>20100201</v>
@@ -6580,7 +6583,7 @@
         <v>1.6800000000000001E-3</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J146">
         <v>20100201</v>
@@ -6621,7 +6624,7 @@
         <v>3.8600000000000001E-3</v>
       </c>
       <c r="G147">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J147">
         <v>20100201</v>
@@ -6703,7 +6706,7 @@
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J149">
         <v>20100201</v>
@@ -6744,7 +6747,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G150">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J150">
         <v>20100201</v>
@@ -6826,7 +6829,7 @@
         <v>6.4900000000000001E-3</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>3.4400000000000001E-4</v>
       </c>
       <c r="J152">
         <v>20100201</v>
@@ -6867,7 +6870,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G153">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J153">
         <v>20100201</v>
@@ -6949,7 +6952,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="G155">
-        <v>0</v>
+        <v>3.14E-3</v>
       </c>
       <c r="J155">
         <v>20100201</v>
@@ -7031,7 +7034,7 @@
         <v>8.8900000000000003E-3</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="J157">
         <v>20100201</v>
@@ -7094,6 +7097,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P158"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes the help menu
</commit_message>
<xml_diff>
--- a/Inputs/ertac_additional_variables.xlsx
+++ b/Inputs/ertac_additional_variables.xlsx
@@ -569,25 +569,28 @@
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fixed the iowa bug and one that occrured if you didn't use the RPO file
</commit_message>
<xml_diff>
--- a/Inputs/ertac_additional_variables.xlsx
+++ b/Inputs/ertac_additional_variables.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLP Valued Customer\Documents\GitHub\ERTAC-EGU-Emission-Projection-Tool\Inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="8595" windowHeight="7740"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="8592" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,8 +241,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +279,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -324,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +369,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +404,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,36 +580,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:P158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -667,7 +682,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J2">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K2">
         <v>62</v>
@@ -685,7 +700,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -726,7 +741,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -767,7 +782,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -808,7 +823,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -831,7 +846,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J6">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K6">
         <v>62</v>
@@ -849,7 +864,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -890,7 +905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -931,7 +946,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -972,7 +987,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1060,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1215,7 +1230,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J15">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K15">
         <v>62</v>
@@ -1233,7 +1248,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1315,7 +1330,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1356,7 +1371,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1397,7 +1412,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1420,7 +1435,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J20">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K20">
         <v>62</v>
@@ -1438,7 +1453,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1561,7 +1576,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1617,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1625,7 +1640,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J25">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K25">
         <v>62</v>
@@ -1643,7 +1658,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1684,7 +1699,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1725,7 +1740,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1766,7 +1781,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J30">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K30">
         <v>62</v>
@@ -1848,7 +1863,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1889,7 +1904,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1930,7 +1945,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1971,7 +1986,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2012,7 +2027,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J35">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K35">
         <v>62</v>
@@ -2053,7 +2068,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2094,7 +2109,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2135,7 +2150,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2176,7 +2191,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -2217,7 +2232,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -2240,7 +2255,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J40">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K40">
         <v>62</v>
@@ -2258,7 +2273,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -2340,7 +2355,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2381,7 +2396,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -2422,7 +2437,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -2445,7 +2460,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J45">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K45">
         <v>62</v>
@@ -2463,7 +2478,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -2545,7 +2560,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -2586,7 +2601,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -2627,7 +2642,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -2650,7 +2665,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J50">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K50">
         <v>62</v>
@@ -2668,7 +2683,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -2709,7 +2724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2750,7 +2765,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2791,7 +2806,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2832,7 +2847,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -2855,7 +2870,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J55">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K55">
         <v>62</v>
@@ -2873,7 +2888,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2914,7 +2929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -2955,7 +2970,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -2996,7 +3011,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -3037,7 +3052,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -3060,7 +3075,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J60">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K60">
         <v>62</v>
@@ -3078,7 +3093,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>39</v>
       </c>
@@ -3119,7 +3134,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -3160,7 +3175,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -3201,7 +3216,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -3242,7 +3257,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -3265,7 +3280,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J65">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K65">
         <v>62</v>
@@ -3283,7 +3298,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>40</v>
       </c>
@@ -3324,7 +3339,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>40</v>
       </c>
@@ -3365,7 +3380,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -3406,7 +3421,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>40</v>
       </c>
@@ -3447,7 +3462,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -3488,7 +3503,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -3529,7 +3544,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -3593,7 +3608,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J73">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K73">
         <v>62</v>
@@ -3611,7 +3626,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -3652,7 +3667,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -3693,7 +3708,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -3734,7 +3749,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -3775,7 +3790,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -3798,7 +3813,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J78">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K78">
         <v>62</v>
@@ -3816,7 +3831,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -3857,7 +3872,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -3898,7 +3913,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -3939,7 +3954,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -3962,7 +3977,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J82">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K82">
         <v>62</v>
@@ -3980,7 +3995,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -4021,7 +4036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -4062,7 +4077,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -4103,7 +4118,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -4126,7 +4141,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J86">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K86">
         <v>62</v>
@@ -4144,7 +4159,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>45</v>
       </c>
@@ -4185,7 +4200,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -4226,7 +4241,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>45</v>
       </c>
@@ -4267,7 +4282,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>45</v>
       </c>
@@ -4308,7 +4323,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>46</v>
       </c>
@@ -4331,7 +4346,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J91">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K91">
         <v>62</v>
@@ -4349,7 +4364,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>46</v>
       </c>
@@ -4390,7 +4405,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>46</v>
       </c>
@@ -4431,7 +4446,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>46</v>
       </c>
@@ -4472,7 +4487,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>46</v>
       </c>
@@ -4513,7 +4528,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -4536,7 +4551,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J96">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K96">
         <v>62</v>
@@ -4554,7 +4569,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -4595,7 +4610,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -4636,7 +4651,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -4677,7 +4692,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -4718,7 +4733,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4759,7 +4774,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -4800,7 +4815,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -4841,7 +4856,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -4882,7 +4897,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>49</v>
       </c>
@@ -4923,7 +4938,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>49</v>
       </c>
@@ -4964,7 +4979,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>49</v>
       </c>
@@ -5005,7 +5020,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>49</v>
       </c>
@@ -5046,7 +5061,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>50</v>
       </c>
@@ -5069,7 +5084,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J109">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K109">
         <v>62</v>
@@ -5087,7 +5102,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>50</v>
       </c>
@@ -5128,7 +5143,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>50</v>
       </c>
@@ -5169,7 +5184,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>50</v>
       </c>
@@ -5210,7 +5225,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>50</v>
       </c>
@@ -5251,7 +5266,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>51</v>
       </c>
@@ -5292,7 +5307,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>51</v>
       </c>
@@ -5333,7 +5348,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>51</v>
       </c>
@@ -5374,7 +5389,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>51</v>
       </c>
@@ -5415,7 +5430,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>52</v>
       </c>
@@ -5438,7 +5453,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J118">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K118">
         <v>62</v>
@@ -5456,7 +5471,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>52</v>
       </c>
@@ -5497,7 +5512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>52</v>
       </c>
@@ -5538,7 +5553,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>52</v>
       </c>
@@ -5579,7 +5594,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>52</v>
       </c>
@@ -5620,7 +5635,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -5643,7 +5658,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J123">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K123">
         <v>62</v>
@@ -5661,7 +5676,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>53</v>
       </c>
@@ -5702,7 +5717,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>53</v>
       </c>
@@ -5743,7 +5758,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>53</v>
       </c>
@@ -5784,7 +5799,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>53</v>
       </c>
@@ -5825,7 +5840,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>54</v>
       </c>
@@ -5869,7 +5884,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -5892,7 +5907,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J129">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K129">
         <v>62</v>
@@ -5910,7 +5925,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>55</v>
       </c>
@@ -5951,7 +5966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>55</v>
       </c>
@@ -5992,7 +6007,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>55</v>
       </c>
@@ -6033,7 +6048,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>55</v>
       </c>
@@ -6074,7 +6089,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>56</v>
       </c>
@@ -6097,7 +6112,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J134">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K134">
         <v>62</v>
@@ -6115,7 +6130,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>56</v>
       </c>
@@ -6156,7 +6171,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>56</v>
       </c>
@@ -6197,7 +6212,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -6238,7 +6253,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>56</v>
       </c>
@@ -6279,7 +6294,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>57</v>
       </c>
@@ -6302,7 +6317,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J139">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K139">
         <v>62</v>
@@ -6320,7 +6335,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>57</v>
       </c>
@@ -6361,7 +6376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>57</v>
       </c>
@@ -6402,7 +6417,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>57</v>
       </c>
@@ -6443,7 +6458,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>57</v>
       </c>
@@ -6484,7 +6499,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>58</v>
       </c>
@@ -6507,7 +6522,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J144">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K144">
         <v>62</v>
@@ -6525,7 +6540,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>58</v>
       </c>
@@ -6566,7 +6581,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>58</v>
       </c>
@@ -6607,7 +6622,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>58</v>
       </c>
@@ -6648,7 +6663,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>58</v>
       </c>
@@ -6689,7 +6704,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -6730,7 +6745,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>60</v>
       </c>
@@ -6753,7 +6768,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J150">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K150">
         <v>62</v>
@@ -6771,7 +6786,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>60</v>
       </c>
@@ -6812,7 +6827,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -6853,7 +6868,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>60</v>
       </c>
@@ -6894,7 +6909,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>60</v>
       </c>
@@ -6935,7 +6950,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>61</v>
       </c>
@@ -6958,7 +6973,7 @@
         <v>3.14E-3</v>
       </c>
       <c r="J155">
-        <v>20100201</v>
+        <v>10100601</v>
       </c>
       <c r="K155">
         <v>62</v>
@@ -6976,7 +6991,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -7017,7 +7032,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>61</v>
       </c>
@@ -7058,7 +7073,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>61</v>
       </c>

</xml_diff>